<commit_message>
Añadiendo cambios de iteración al leer archivo de excel
</commit_message>
<xml_diff>
--- a/DataDrive/Products.xlsx
+++ b/DataDrive/Products.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmanuel.escobar\eclipse-workspace\testBuyingProducts\DataDrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{54C8A3CA-E6EF-45EC-9501-C25CCA942F06}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{496C0860-CEED-4236-82FE-DC224ACE679B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20628" windowHeight="7764" xr2:uid="{CDCF97F6-056B-4B73-BC3B-44B20D02336A}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>MacBook</t>
   </si>
   <si>
     <t>iPhone</t>
-  </si>
-  <si>
-    <t>Canon EOS 5D</t>
   </si>
   <si>
     <t>Samsung Galaxy Tab 10.1</t>
@@ -388,18 +385,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7005CC-C550-45C0-8442-844A48CE5466}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,9 +407,6 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>